<commit_message>
Rearranged stats output. Split downloads into classic vs next gen by country
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\apsim-downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FD1F33-6A92-4052-AD6D-EC21DFB77660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DA8C47-598F-429E-81D5-558684EB8E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="880" windowWidth="23920" windowHeight="11620" xr2:uid="{C6F40090-B944-4A19-85BA-B0BCA541DE98}"/>
+    <workbookView xWindow="13240" yWindow="880" windowWidth="17910" windowHeight="11620" xr2:uid="{C6F40090-B944-4A19-85BA-B0BCA541DE98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>APSIM Next Generation</t>
   </si>
   <si>
     <t>APSIM 7.x</t>
@@ -81,7 +78,46 @@
     <t>2021-22</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>NumDownloads</t>
+  </si>
+  <si>
+    <t>NumRegistrations</t>
+  </si>
+  <si>
+    <t>NumUpgrades</t>
+  </si>
+  <si>
+    <t>NumCountries</t>
+  </si>
+  <si>
+    <t>AUDownloadsClassic</t>
+  </si>
+  <si>
+    <t>AUDownloadsNextGen</t>
+  </si>
+  <si>
+    <t>NZDownloadsClassic</t>
+  </si>
+  <si>
+    <t>NZDownloadsNextGen</t>
+  </si>
+  <si>
+    <t>ChinaDownloadsNextGen</t>
+  </si>
+  <si>
+    <t>AfricaDownloadsNextGen</t>
+  </si>
+  <si>
+    <t>Next Gen.</t>
+  </si>
+  <si>
+    <t>Total USA</t>
+  </si>
+  <si>
+    <t>US APSIM 7.x</t>
+  </si>
+  <si>
+    <t>US NextGen.</t>
   </si>
 </sst>
 </file>
@@ -179,7 +215,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -242,7 +278,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Sheet1!$F$2:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -293,11 +329,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>APSIM Next Generation</c:v>
+                  <c:v>Next Gen.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -356,7 +392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$G$2:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -399,6 +435,906 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BAA5-4751-8001-34F7091D6A6F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1155200160"/>
+        <c:axId val="1155221792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1155200160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155221792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1155221792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155200160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>USA</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>US APSIM 7.x</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$2:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>337</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>152</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7943-4194-941E-9DA4368B1BBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>US NextGen.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$2:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>358</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7943-4194-941E-9DA4368B1BBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1155200160"/>
+        <c:axId val="1155221792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1155200160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155221792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1155221792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155200160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>USA</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total USA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>192</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>401</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>510</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A127-44D0-8B39-7FC39FCB17CC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -645,6 +1581,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1148,19 +2164,1025 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1181,6 +3203,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B62084BD-4C7B-43A3-99A9-8ED1E69FDFBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1238250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB49048C-B52A-400A-A5C1-530BE3D700AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1486,38 +3584,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4F10B0-D811-4319-9945-30AEFBBB37B9}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="4" max="4" width="22.90625" customWidth="1"/>
+    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>2012</v>
@@ -1526,16 +3679,58 @@
         <v>1296</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1296</v>
       </c>
       <c r="E2">
-        <f>SUM(C2:D2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>1296</v>
       </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>82</v>
+      </c>
+      <c r="I2">
+        <v>302</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>41</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>64</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>89</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>M2+N2</f>
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B12" si="0">B2+1</f>
@@ -1545,12 +3740,58 @@
         <v>1475</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1475</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1475</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>105</v>
+      </c>
+      <c r="I3">
+        <v>339</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>37</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>98</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>113</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S12" si="1">M3+N3</f>
+        <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
@@ -1560,12 +3801,58 @@
         <v>1712</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1712</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1712</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>98</v>
+      </c>
+      <c r="I4">
+        <v>438</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>26</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>102</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>154</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="1"/>
+        <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
@@ -1575,112 +3862,480 @@
         <v>2002</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2002</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>2002</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>112</v>
+      </c>
+      <c r="I5">
+        <v>462</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>51</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>174</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>123</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
       <c r="C6">
+        <v>2379</v>
+      </c>
+      <c r="D6">
+        <v>2309</v>
+      </c>
+      <c r="E6">
+        <v>70</v>
+      </c>
+      <c r="F6">
         <v>2150</v>
       </c>
-      <c r="D6">
+      <c r="G6">
         <v>106</v>
       </c>
+      <c r="H6">
+        <v>106</v>
+      </c>
+      <c r="I6">
+        <v>547</v>
+      </c>
+      <c r="J6">
+        <v>71</v>
+      </c>
+      <c r="K6">
+        <v>19</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>180</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>215</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>2017</v>
       </c>
       <c r="C7">
+        <v>2937</v>
+      </c>
+      <c r="D7">
+        <v>2531</v>
+      </c>
+      <c r="E7">
+        <v>406</v>
+      </c>
+      <c r="F7">
         <v>2391</v>
       </c>
-      <c r="D7">
+      <c r="G7">
         <v>500</v>
       </c>
+      <c r="H7">
+        <v>112</v>
+      </c>
+      <c r="I7">
+        <v>602</v>
+      </c>
+      <c r="J7">
+        <v>324</v>
+      </c>
+      <c r="K7">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>28</v>
+      </c>
+      <c r="M7">
+        <v>168</v>
+      </c>
+      <c r="N7">
+        <v>24</v>
+      </c>
+      <c r="O7">
+        <v>290</v>
+      </c>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
       <c r="C8">
+        <v>3672</v>
+      </c>
+      <c r="D8">
+        <v>3107</v>
+      </c>
+      <c r="E8">
+        <v>565</v>
+      </c>
+      <c r="F8">
         <v>2890</v>
       </c>
-      <c r="D8">
+      <c r="G8">
         <v>782</v>
       </c>
+      <c r="H8">
+        <v>110</v>
+      </c>
+      <c r="I8">
+        <v>653</v>
+      </c>
+      <c r="J8">
+        <v>480</v>
+      </c>
+      <c r="K8">
+        <v>47</v>
+      </c>
+      <c r="L8">
+        <v>69</v>
+      </c>
+      <c r="M8">
+        <v>211</v>
+      </c>
+      <c r="N8">
+        <v>34</v>
+      </c>
+      <c r="O8">
+        <v>307</v>
+      </c>
+      <c r="P8">
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="1"/>
+        <v>245</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
       <c r="C9">
+        <v>4172</v>
+      </c>
+      <c r="D9">
+        <v>3702</v>
+      </c>
+      <c r="E9">
+        <v>469</v>
+      </c>
+      <c r="F9">
         <v>3304</v>
       </c>
-      <c r="D9">
+      <c r="G9">
         <v>866</v>
       </c>
+      <c r="H9">
+        <v>110</v>
+      </c>
+      <c r="I9">
+        <v>749</v>
+      </c>
+      <c r="J9">
+        <v>568</v>
+      </c>
+      <c r="K9">
+        <v>36</v>
+      </c>
+      <c r="L9">
+        <v>42</v>
+      </c>
+      <c r="M9">
+        <v>337</v>
+      </c>
+      <c r="N9">
+        <v>33</v>
+      </c>
+      <c r="O9">
+        <v>410</v>
+      </c>
+      <c r="P9">
+        <v>23</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
       <c r="C10">
+        <v>4653</v>
+      </c>
+      <c r="D10">
+        <v>3792</v>
+      </c>
+      <c r="E10">
+        <v>861</v>
+      </c>
+      <c r="F10">
         <v>2986</v>
       </c>
-      <c r="D10">
+      <c r="G10">
         <v>1667</v>
       </c>
+      <c r="H10">
+        <v>118</v>
+      </c>
+      <c r="I10">
+        <v>800</v>
+      </c>
+      <c r="J10">
+        <v>901</v>
+      </c>
+      <c r="K10">
+        <v>43</v>
+      </c>
+      <c r="L10">
+        <v>179</v>
+      </c>
+      <c r="M10">
+        <v>246</v>
+      </c>
+      <c r="N10">
+        <v>84</v>
+      </c>
+      <c r="O10">
+        <v>399</v>
+      </c>
+      <c r="P10">
+        <v>36</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
       <c r="C11">
+        <v>5699</v>
+      </c>
+      <c r="D11">
+        <v>4702</v>
+      </c>
+      <c r="E11">
+        <v>997</v>
+      </c>
+      <c r="F11">
         <v>3880</v>
       </c>
-      <c r="D11">
+      <c r="G11">
         <v>1819</v>
       </c>
+      <c r="H11">
+        <v>132</v>
+      </c>
+      <c r="I11">
+        <v>771</v>
+      </c>
+      <c r="J11">
+        <v>820</v>
+      </c>
+      <c r="K11">
+        <v>94</v>
+      </c>
+      <c r="L11">
+        <v>112</v>
+      </c>
+      <c r="M11">
+        <v>293</v>
+      </c>
+      <c r="N11">
+        <v>108</v>
+      </c>
+      <c r="O11">
+        <v>573</v>
+      </c>
+      <c r="P11">
+        <v>151</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="1"/>
+        <v>401</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
       <c r="C12">
+        <v>6649</v>
+      </c>
+      <c r="D12">
+        <v>3338</v>
+      </c>
+      <c r="E12">
+        <v>3311</v>
+      </c>
+      <c r="F12">
         <v>1856</v>
       </c>
-      <c r="D12">
+      <c r="G12">
         <v>4008</v>
+      </c>
+      <c r="H12">
+        <v>114</v>
+      </c>
+      <c r="I12">
+        <v>394</v>
+      </c>
+      <c r="J12">
+        <v>1636</v>
+      </c>
+      <c r="K12">
+        <v>23</v>
+      </c>
+      <c r="L12">
+        <v>58</v>
+      </c>
+      <c r="M12">
+        <v>152</v>
+      </c>
+      <c r="N12">
+        <v>358</v>
+      </c>
+      <c r="O12">
+        <v>393</v>
+      </c>
+      <c r="P12">
+        <v>435</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>